<commit_message>
Iran and canada predictions updated
</commit_message>
<xml_diff>
--- a/future_prediction/canada/Weekly-Deaths-Prediction r = 1.xlsx
+++ b/future_prediction/canada/Weekly-Deaths-Prediction r = 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="58">
   <si>
     <t>the day the prediction is made</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>03 Jan -- 09 Jan 2021</t>
+  </si>
+  <si>
+    <t>10 Jan -- 16 Jan 2021</t>
   </si>
   <si>
     <t>KNN</t>
@@ -542,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G2">
         <v>1.27</v>
@@ -629,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -649,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -669,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -689,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -709,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -729,7 +732,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -749,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -769,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -789,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -809,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -829,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -849,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -869,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -889,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -909,7 +912,7 @@
         <v>4.67</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -929,7 +932,7 @@
         <v>7.06</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -949,7 +952,7 @@
         <v>5.83</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -969,7 +972,7 @@
         <v>8.69</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -989,7 +992,7 @@
         <v>4.95</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1009,7 +1012,7 @@
         <v>7.13</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1029,7 +1032,7 @@
         <v>2.95</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1049,7 +1052,7 @@
         <v>2.83</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1069,7 +1072,7 @@
         <v>1.32</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1089,7 +1092,7 @@
         <v>2.52</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1109,7 +1112,7 @@
         <v>3.01</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1129,7 +1132,7 @@
         <v>0.06</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1149,7 +1152,7 @@
         <v>0.24</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1169,7 +1172,7 @@
         <v>17.92</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1189,7 +1192,7 @@
         <v>68.53</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1209,7 +1212,7 @@
         <v>0.51</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1229,7 +1232,7 @@
         <v>15.46</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1249,7 +1252,7 @@
         <v>6.64</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1269,7 +1272,7 @@
         <v>9.550000000000001</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1289,7 +1292,7 @@
         <v>7.23</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1309,7 +1312,7 @@
         <v>17.01</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1329,7 +1332,7 @@
         <v>6.1</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1349,7 +1352,7 @@
         <v>4.42</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1369,7 +1372,7 @@
         <v>8.470000000000001</v>
       </c>
       <c r="F40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1389,7 +1392,7 @@
         <v>3.18</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1409,7 +1412,7 @@
         <v>18.29</v>
       </c>
       <c r="F42" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -1429,7 +1432,7 @@
         <v>38.18</v>
       </c>
       <c r="F43" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -1449,7 +1452,7 @@
         <v>61.88</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J44">
         <v>61.88</v>
@@ -1475,13 +1478,27 @@
         <v>61.88</v>
       </c>
       <c r="F45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J45">
         <v>61.88</v>
       </c>
       <c r="K45">
         <v>37.28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46">
+        <v>116.14</v>
+      </c>
+      <c r="F46" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>